<commit_message>
Calculo do angulo de extinção
</commit_message>
<xml_diff>
--- a/Exp2/dados/Pasta1.xlsx
+++ b/Exp2/dados/Pasta1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">R</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t xml:space="preserve">rms teórica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angulo Extincao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angulo Rad</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,6 +293,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -377,7 +387,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -413,7 +423,7 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Carga RL</a:t>
+              <a:t>Carga R</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -430,7 +440,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$F$2</c:f>
+              <c:f>g!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -454,6 +464,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -529,7 +540,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$F$3:$F$21</c:f>
+              <c:f>g!$B$3:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -540,55 +551,55 @@
                   <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -600,7 +611,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$H$2</c:f>
+              <c:f>g!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -624,6 +635,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -699,12 +711,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$H$3:$H$21</c:f>
+              <c:f>g!$D$3:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>120.920914641885</c:v>
+                  <c:v>120.920914651219</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>120.038946692024</c:v>
@@ -770,7 +782,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$G$2</c:f>
+              <c:f>g!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -794,6 +806,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -869,7 +882,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$G$3:$G$21</c:f>
+              <c:f>g!$C$3:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -880,7 +893,7 @@
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>131</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>130</c:v>
@@ -901,19 +914,19 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>93</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>73</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>61</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>50</c:v>
@@ -925,10 +938,10 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -940,7 +953,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$I$2</c:f>
+              <c:f>g!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -964,6 +977,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1039,12 +1053,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$I$3:$I$21</c:f>
+              <c:f>g!$E$3:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>134.350245771435</c:v>
+                  <c:v>134.349682269024</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>134.2749398365</c:v>
@@ -1105,11 +1119,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="11335368"/>
-        <c:axId val="15074347"/>
+        <c:axId val="19078818"/>
+        <c:axId val="59665933"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11335368"/>
+        <c:axId val="19078818"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1183,12 +1197,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15074347"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="59665933"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15074347"/>
+        <c:axId val="59665933"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11335368"/>
+        <c:crossAx val="19078818"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1307,7 +1321,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1343,7 +1357,7 @@
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Carga R</a:t>
+              <a:t>Carga RL</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1360,7 +1374,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$B$2</c:f>
+              <c:f>g!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1460,7 +1474,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$B$3:$B$21</c:f>
+              <c:f>g!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1471,55 +1485,55 @@
                   <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>111</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,7 +1545,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$D$2</c:f>
+              <c:f>g!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1631,66 +1645,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$D$3:$D$21</c:f>
+              <c:f>g!$H$3:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>120.920914651219</c:v>
+                  <c:v>120.884072552598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120.038946692024</c:v>
+                  <c:v>119.120136634208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.310434097241</c:v>
+                  <c:v>113.663111444642</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>112.855123439991</c:v>
+                  <c:v>104.752490130141</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106.808387080096</c:v>
+                  <c:v>92.6590174103523</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99.3539520420581</c:v>
+                  <c:v>77.7501473342758</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.7183175623804</c:v>
+                  <c:v>60.4788783749203</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.1638730248862</c:v>
+                  <c:v>52.2382433781639</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70.9809253920651</c:v>
+                  <c:v>44.085270010222</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60.4788783749202</c:v>
+                  <c:v>35.9532310301402</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.9768313577754</c:v>
+                  <c:v>28.1469491454805</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>39.7938837249543</c:v>
+                  <c:v>20.9524729030146</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30.2394391874601</c:v>
+                  <c:v>14.6217199821216</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.6038047077823</c:v>
+                  <c:v>9.35585130424909</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.1493696697441</c:v>
+                  <c:v>5.28715595228338</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.10263330984998</c:v>
+                  <c:v>2.4589744854984</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.64732265259924</c:v>
+                  <c:v>0.802757211154487</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.918810057816419</c:v>
+                  <c:v>0.110583125008187</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.036842098621395</c:v>
+                  <c:v>0.000956933143054376</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1702,7 +1716,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$C$2</c:f>
+              <c:f>g!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1802,7 +1816,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$C$3:$C$21</c:f>
+              <c:f>g!$G$3:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1813,7 +1827,7 @@
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>130</c:v>
@@ -1834,19 +1848,19 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>101</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>72</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>60</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>50</c:v>
@@ -1858,10 +1872,10 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1873,7 +1887,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>g!$E$2</c:f>
+              <c:f>g!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1973,77 +1987,77 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>g!$E$3:$E$21</c:f>
+              <c:f>g!$I$3:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>134.349682269024</c:v>
+                  <c:v>135.464571368764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>134.2749398365</c:v>
+                  <c:v>139.754729720277</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133.75728183405</c:v>
+                  <c:v>144.496031935353</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>132.399162789111</c:v>
+                  <c:v>148.237124236796</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>129.876834477713</c:v>
+                  <c:v>150.750354043536</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.95719255435</c:v>
+                  <c:v>151.920225475604</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.503962482253</c:v>
+                  <c:v>151.742358229934</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113.4774054812</c:v>
+                  <c:v>145.600053625674</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104.930048240012</c:v>
+                  <c:v>137.992859142461</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95</c:v>
+                  <c:v>129.237591199242</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>83.9028305621976</c:v>
+                  <c:v>119.545688066766</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71.9227255132576</c:v>
+                  <c:v>109.1716900734</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>59.4036617227914</c:v>
+                  <c:v>98.3815201288035</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>46.7416906393688</c:v>
+                  <c:v>87.4030263833</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.3803412730107</c:v>
+                  <c:v>76.3465339978088</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.8136295389948</c:v>
+                  <c:v>65.0695421688352</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.6091060891129</c:v>
+                  <c:v>52.9037565557211</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.4989478663791</c:v>
+                  <c:v>37.797845555041</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.403576773894424</c:v>
+                  <c:v>17.2349536924222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61076173"/>
-        <c:axId val="30855084"/>
+        <c:axId val="86286457"/>
+        <c:axId val="17831062"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61076173"/>
+        <c:axId val="86286457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2117,12 +2131,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30855084"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="17831062"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30855084"/>
+        <c:axId val="17831062"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2218,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61076173"/>
+        <c:crossAx val="86286457"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2248,13 +2262,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>88920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>555120</xdr:colOff>
+      <xdr:colOff>554760</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>106920</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2263,7 +2277,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="88920" y="3884760"/>
-        <a:ext cx="5761800" cy="3232440"/>
+        <a:ext cx="5761440" cy="3232080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2275,16 +2289,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>337680</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>558360</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>565200</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2292,8 +2306,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6064560" y="3855960"/>
-        <a:ext cx="5761800" cy="3232440"/>
+        <a:off x="7595640" y="3972600"/>
+        <a:ext cx="5761440" cy="3232080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2311,10 +2325,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2371,8 +2385,14 @@
       <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <v>2</v>
       </c>
@@ -2397,15 +2417,22 @@
         <v>131</v>
       </c>
       <c r="H3" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H24)+ COS(A3*PI()/180))/PI()</f>
-        <v>120.920914641885</v>
+        <f aca="false">190*(-COS(PI() + J3)+ COS(A3*PI()/180))/PI()</f>
+        <v>120.884072552598</v>
       </c>
       <c r="I3" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H24 - SIN(PI() + H24)/2 + SIN(2*A3*PI()/180)/2 - A3*PI()/180))/SQRT(2*PI())</f>
-        <v>134.350245771435</v>
+        <f aca="false">(190*SQRT(PI() + J3 - SIN(PI() + J3)/2 + SIN(2*A3*PI()/180)/2 - A3*PI()/180))/SQRT(2*PI())</f>
+        <v>135.464571368764</v>
+      </c>
+      <c r="J3" s="12" t="n">
+        <v>0.034906585039887</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">A3*PI()/180</f>
+        <v>0.0349065850398866</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="n">
         <v>10</v>
       </c>
@@ -2430,12 +2457,19 @@
         <v>131</v>
       </c>
       <c r="H4" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H25)+ COS(A4*PI()/180))/PI()</f>
-        <v>120.038946692024</v>
+        <f aca="false">190*(-COS(PI() + J4)+ COS(A4*PI()/180))/PI()</f>
+        <v>119.120136634208</v>
       </c>
       <c r="I4" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H25 - SIN(PI() + H25)/2 + SIN(2*A4*PI()/180)/2 - A4*PI()/180))/SQRT(2*PI())</f>
-        <v>134.2749398365</v>
+        <f aca="false">(190*SQRT(PI() + J4 - SIN(PI() + J4)/2 + SIN(2*A4*PI()/180)/2 - A4*PI()/180))/SQRT(2*PI())</f>
+        <v>139.754729720277</v>
+      </c>
+      <c r="J4" s="12" t="n">
+        <v>0.174532925199433</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">A4*PI()/180</f>
+        <v>0.174532925199433</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,12 +2497,19 @@
         <v>131</v>
       </c>
       <c r="H5" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H26)+ COS(A5*PI()/180))/PI()</f>
-        <v>117.310434097241</v>
+        <f aca="false">190*(-COS(PI() + J5)+ COS(A5*PI()/180))/PI()</f>
+        <v>113.663111444642</v>
       </c>
       <c r="I5" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H26 - SIN(PI() + H26)/2 + SIN(2*A5*PI()/180)/2 - A5*PI()/180))/SQRT(2*PI())</f>
-        <v>133.75728183405</v>
+        <f aca="false">(190*SQRT(PI() + J5 - SIN(PI() + J5)/2 + SIN(2*A5*PI()/180)/2 - A5*PI()/180))/SQRT(2*PI())</f>
+        <v>144.496031935353</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.349065850398866</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">A5*PI()/180</f>
+        <v>0.349065850398866</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,12 +2537,19 @@
         <v>130</v>
       </c>
       <c r="H6" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H27)+ COS(A6*PI()/180))/PI()</f>
-        <v>112.855123439991</v>
+        <f aca="false">190*(-COS(PI() + J6)+ COS(A6*PI()/180))/PI()</f>
+        <v>104.752490130141</v>
       </c>
       <c r="I6" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H27 - SIN(PI() + H27)/2 + SIN(2*A6*PI()/180)/2 - A6*PI()/180))/SQRT(2*PI())</f>
-        <v>132.399162789111</v>
+        <f aca="false">(190*SQRT(PI() + J6 - SIN(PI() + J6)/2 + SIN(2*A6*PI()/180)/2 - A6*PI()/180))/SQRT(2*PI())</f>
+        <v>148.237124236796</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.523598775598299</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">A6*PI()/180</f>
+        <v>0.523598775598299</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,12 +2577,19 @@
         <v>128</v>
       </c>
       <c r="H7" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H28)+ COS(A7*PI()/180))/PI()</f>
-        <v>106.808387080096</v>
+        <f aca="false">190*(-COS(PI() + J7)+ COS(A7*PI()/180))/PI()</f>
+        <v>92.6590174103523</v>
       </c>
       <c r="I7" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H28 - SIN(PI() + H28)/2 + SIN(2*A7*PI()/180)/2 - A7*PI()/180))/SQRT(2*PI())</f>
-        <v>129.876834477713</v>
+        <f aca="false">(190*SQRT(PI() + J7 - SIN(PI() + J7)/2 + SIN(2*A7*PI()/180)/2 - A7*PI()/180))/SQRT(2*PI())</f>
+        <v>150.750354043536</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.698131700797732</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">A7*PI()/180</f>
+        <v>0.698131700797732</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,12 +2617,19 @@
         <v>125</v>
       </c>
       <c r="H8" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H29)+ COS(A8*PI()/180))/PI()</f>
-        <v>99.3539520420581</v>
+        <f aca="false">190*(-COS(PI() + J8)+ COS(A8*PI()/180))/PI()</f>
+        <v>77.7501473342758</v>
       </c>
       <c r="I8" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H29 - SIN(PI() + H29)/2 + SIN(2*A8*PI()/180)/2 - A8*PI()/180))/SQRT(2*PI())</f>
-        <v>125.95719255435</v>
+        <f aca="false">(190*SQRT(PI() + J8 - SIN(PI() + J8)/2 + SIN(2*A8*PI()/180)/2 - A8*PI()/180))/SQRT(2*PI())</f>
+        <v>151.920225475604</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.872664625997165</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">A8*PI()/180</f>
+        <v>0.872664625997165</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,12 +2657,19 @@
         <v>121</v>
       </c>
       <c r="H9" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H30)+ COS(A9*PI()/180))/PI()</f>
-        <v>90.7183175623804</v>
+        <f aca="false">190*(-COS(PI() + J9)+ COS(A9*PI()/180))/PI()</f>
+        <v>60.4788783749203</v>
       </c>
       <c r="I9" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H30 - SIN(PI() + H30)/2 + SIN(2*A9*PI()/180)/2 - A9*PI()/180))/SQRT(2*PI())</f>
-        <v>120.503962482253</v>
+        <f aca="false">(190*SQRT(PI() + J9 - SIN(PI() + J9)/2 + SIN(2*A9*PI()/180)/2 - A9*PI()/180))/SQRT(2*PI())</f>
+        <v>151.742358229934</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1.0471975511966</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">A9*PI()/180</f>
+        <v>1.0471975511966</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,12 +2697,19 @@
         <v>115</v>
       </c>
       <c r="H10" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H31)+ COS(A10*PI()/180))/PI()</f>
-        <v>81.1638730248862</v>
+        <f aca="false">190*(-COS(PI() + J10)+ COS(A10*PI()/180))/PI()</f>
+        <v>52.2382433781639</v>
       </c>
       <c r="I10" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H31 - SIN(PI() + H31)/2 + SIN(2*A10*PI()/180)/2 - A10*PI()/180))/SQRT(2*PI())</f>
-        <v>113.4774054812</v>
+        <f aca="false">(190*SQRT(PI() + J10 - SIN(PI() + J10)/2 + SIN(2*A10*PI()/180)/2 - A10*PI()/180))/SQRT(2*PI())</f>
+        <v>145.600053625674</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1.02192644225211</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">A10*PI()/180</f>
+        <v>1.22173047639603</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,12 +2737,19 @@
         <v>108</v>
       </c>
       <c r="H11" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H32)+ COS(A11*PI()/180))/PI()</f>
-        <v>70.9809253920651</v>
+        <f aca="false">190*(-COS(PI() + J11)+ COS(A11*PI()/180))/PI()</f>
+        <v>44.085270010222</v>
       </c>
       <c r="I11" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H32 - SIN(PI() + H32)/2 + SIN(2*A11*PI()/180)/2 - A11*PI()/180))/SQRT(2*PI())</f>
-        <v>104.930048240012</v>
+        <f aca="false">(190*SQRT(PI() + J11 - SIN(PI() + J11)/2 + SIN(2*A11*PI()/180)/2 - A11*PI()/180))/SQRT(2*PI())</f>
+        <v>137.992859142461</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.982086556239764</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">A11*PI()/180</f>
+        <v>1.39626340159546</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,12 +2777,19 @@
         <v>100</v>
       </c>
       <c r="H12" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H33)+ COS(A12*PI()/180))/PI()</f>
-        <v>60.4788783749202</v>
+        <f aca="false">190*(-COS(PI() + J12)+ COS(A12*PI()/180))/PI()</f>
+        <v>35.9532310301402</v>
       </c>
       <c r="I12" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H33 - SIN(PI() + H33)/2 + SIN(2*A12*PI()/180)/2 - A12*PI()/180))/SQRT(2*PI())</f>
-        <v>95</v>
+        <f aca="false">(190*SQRT(PI() + J12 - SIN(PI() + J12)/2 + SIN(2*A12*PI()/180)/2 - A12*PI()/180))/SQRT(2*PI())</f>
+        <v>129.237591199242</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.93418270402243</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">A12*PI()/180</f>
+        <v>1.5707963267949</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,12 +2817,19 @@
         <v>93</v>
       </c>
       <c r="H13" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H34)+ COS(A13*PI()/180))/PI()</f>
-        <v>49.9768313577754</v>
+        <f aca="false">190*(-COS(PI() + J13)+ COS(A13*PI()/180))/PI()</f>
+        <v>28.1469491454805</v>
       </c>
       <c r="I13" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H34 - SIN(PI() + H34)/2 + SIN(2*A13*PI()/180)/2 - A13*PI()/180))/SQRT(2*PI())</f>
-        <v>83.9028305621976</v>
+        <f aca="false">(190*SQRT(PI() + J13 - SIN(PI() + J13)/2 + SIN(2*A13*PI()/180)/2 - A13*PI()/180))/SQRT(2*PI())</f>
+        <v>119.545688066766</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0.877534468892555</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">A13*PI()/180</f>
+        <v>1.74532925199433</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2760,12 +2857,19 @@
         <v>83</v>
       </c>
       <c r="H14" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H35)+ COS(A14*PI()/180))/PI()</f>
-        <v>39.7938837249543</v>
+        <f aca="false">190*(-COS(PI() + J14)+ COS(A14*PI()/180))/PI()</f>
+        <v>20.9524729030146</v>
       </c>
       <c r="I14" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H35 - SIN(PI() + H35)/2 + SIN(2*A14*PI()/180)/2 - A14*PI()/180))/SQRT(2*PI())</f>
-        <v>71.9227255132576</v>
+        <f aca="false">(190*SQRT(PI() + J14 - SIN(PI() + J14)/2 + SIN(2*A14*PI()/180)/2 - A14*PI()/180))/SQRT(2*PI())</f>
+        <v>109.1716900734</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0.811428674750211</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">A14*PI()/180</f>
+        <v>1.91986217719376</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,12 +2897,19 @@
         <v>73</v>
       </c>
       <c r="H15" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H36)+ COS(A15*PI()/180))/PI()</f>
-        <v>30.2394391874601</v>
+        <f aca="false">190*(-COS(PI() + J15)+ COS(A15*PI()/180))/PI()</f>
+        <v>14.6217199821216</v>
       </c>
       <c r="I15" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H36 - SIN(PI() + H36)/2 + SIN(2*A15*PI()/180)/2 - A15*PI()/180))/SQRT(2*PI())</f>
-        <v>59.4036617227914</v>
+        <f aca="false">(190*SQRT(PI() + J15 - SIN(PI() + J15)/2 + SIN(2*A15*PI()/180)/2 - A15*PI()/180))/SQRT(2*PI())</f>
+        <v>98.3815201288035</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0.735096964555009</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">A15*PI()/180</f>
+        <v>2.0943951023932</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,12 +2937,19 @@
         <v>61</v>
       </c>
       <c r="H16" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H37)+ COS(A16*PI()/180))/PI()</f>
-        <v>21.6038047077823</v>
+        <f aca="false">190*(-COS(PI() + J16)+ COS(A16*PI()/180))/PI()</f>
+        <v>9.35585130424909</v>
       </c>
       <c r="I16" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H37 - SIN(PI() + H37)/2 + SIN(2*A16*PI()/180)/2 - A16*PI()/180))/SQRT(2*PI())</f>
-        <v>46.7416906393688</v>
+        <f aca="false">(190*SQRT(PI() + J16 - SIN(PI() + J16)/2 + SIN(2*A16*PI()/180)/2 - A16*PI()/180))/SQRT(2*PI())</f>
+        <v>87.4030263833</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0.647683149376233</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">A16*PI()/180</f>
+        <v>2.26892802759263</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,12 +2977,19 @@
         <v>50</v>
       </c>
       <c r="H17" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H38)+ COS(A17*PI()/180))/PI()</f>
-        <v>14.1493696697441</v>
+        <f aca="false">190*(-COS(PI() + J17)+ COS(A17*PI()/180))/PI()</f>
+        <v>5.28715595228338</v>
       </c>
       <c r="I17" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H38 - SIN(PI() + H38)/2 + SIN(2*A17*PI()/180)/2 - A17*PI()/180))/SQRT(2*PI())</f>
-        <v>34.3803412730107</v>
+        <f aca="false">(190*SQRT(PI() + J17 - SIN(PI() + J17)/2 + SIN(2*A17*PI()/180)/2 - A17*PI()/180))/SQRT(2*PI())</f>
+        <v>76.3465339978088</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0.548196174750787</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">A17*PI()/180</f>
+        <v>2.44346095279206</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,12 +3017,19 @@
         <v>38</v>
       </c>
       <c r="H18" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H39)+ COS(A18*PI()/180))/PI()</f>
-        <v>8.10263330984998</v>
+        <f aca="false">190*(-COS(PI() + J18)+ COS(A18*PI()/180))/PI()</f>
+        <v>2.4589744854984</v>
       </c>
       <c r="I18" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H39 - SIN(PI() + H39)/2 + SIN(2*A18*PI()/180)/2 - A18*PI()/180))/SQRT(2*PI())</f>
-        <v>22.8136295389948</v>
+        <f aca="false">(190*SQRT(PI() + J18 - SIN(PI() + J18)/2 + SIN(2*A18*PI()/180)/2 - A18*PI()/180))/SQRT(2*PI())</f>
+        <v>65.0695421688352</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0.435441728780333</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">A18*PI()/180</f>
+        <v>2.61799387799149</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,12 +3057,19 @@
         <v>27</v>
       </c>
       <c r="H19" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H40)+ COS(A19*PI()/180))/PI()</f>
-        <v>3.64732265259924</v>
+        <f aca="false">190*(-COS(PI() + J19)+ COS(A19*PI()/180))/PI()</f>
+        <v>0.802757211154487</v>
       </c>
       <c r="I19" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H40 - SIN(PI() + H40)/2 + SIN(2*A19*PI()/180)/2 - A19*PI()/180))/SQRT(2*PI())</f>
-        <v>12.6091060891129</v>
+        <f aca="false">(190*SQRT(PI() + J19 - SIN(PI() + J19)/2 + SIN(2*A19*PI()/180)/2 - A19*PI()/180))/SQRT(2*PI())</f>
+        <v>52.9037565557211</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.307920205634587</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">A19*PI()/180</f>
+        <v>2.79252680319093</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,22 +3097,29 @@
         <v>19</v>
       </c>
       <c r="H20" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H41)+ COS(A20*PI()/180))/PI()</f>
-        <v>0.918810057816419</v>
+        <f aca="false">190*(-COS(PI() + J20)+ COS(A20*PI()/180))/PI()</f>
+        <v>0.110583125008187</v>
       </c>
       <c r="I20" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H41 - SIN(PI() + H41)/2 + SIN(2*A20*PI()/180)/2 - A20*PI()/180))/SQRT(2*PI())</f>
-        <v>4.4989478663791</v>
+        <f aca="false">(190*SQRT(PI() + J20 - SIN(PI() + J20)/2 + SIN(2*A20*PI()/180)/2 - A20*PI()/180))/SQRT(2*PI())</f>
+        <v>37.797845555041</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.163668323529781</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">A20*PI()/180</f>
+        <v>2.96705972839036</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="n">
+      <c r="A21" s="13" t="n">
         <v>178</v>
       </c>
-      <c r="B21" s="13" t="n">
+      <c r="B21" s="14" t="n">
         <v>2.5</v>
       </c>
-      <c r="C21" s="14" t="n">
+      <c r="C21" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D21" s="10" t="n">
@@ -2984,25 +3130,32 @@
         <f aca="false">(190*SQRT(PI() + SIN(2*A21*PI()/180)/2 - A21*PI()/180))/SQRT(2*PI())</f>
         <v>0.403576773894424</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="F21" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="14" t="n">
+      <c r="G21" s="15" t="n">
         <v>11</v>
       </c>
       <c r="H21" s="0" t="n">
-        <f aca="false">190*(-COS(PI() + H42)+ COS(A21*PI()/180))/PI()</f>
-        <v>0.036842098621395</v>
+        <f aca="false">190*(-COS(PI() + J21)+ COS(A21*PI()/180))/PI()</f>
+        <v>0.000956933143054376</v>
       </c>
       <c r="I21" s="0" t="n">
-        <f aca="false">(190*SQRT(PI() + H42 - SIN(PI() + H42)/2 + SIN(2*A21*PI()/180)/2 - A21*PI()/180))/SQRT(2*PI())</f>
-        <v>0.403576773894424</v>
+        <f aca="false">(190*SQRT(PI() + J21 - SIN(PI() + J21)/2 + SIN(2*A21*PI()/180)/2 - A21*PI()/180))/SQRT(2*PI())</f>
+        <v>17.2349536924222</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0.0344502269060808</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">A21*PI()/180</f>
+        <v>3.10668606854991</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H24" s="0" t="n">
-        <f aca="false">ATAN((43.9*60*2*PI()/1000000000)/0.942)</f>
-        <v>1.75689066851467E-005</v>
+        <f aca="false">ATAN((43.9*60*2*PI()/1000)/9.42)</f>
+        <v>1.05334135573322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extincao teorico lampada de 57 ohms
</commit_message>
<xml_diff>
--- a/Exp2/dados/Pasta1.xlsx
+++ b/Exp2/dados/Pasta1.xlsx
@@ -22,12 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t xml:space="preserve">R</t>
   </si>
   <si>
     <t xml:space="preserve">RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RL Lampada 57 Ohm</t>
   </si>
   <si>
     <t xml:space="preserve">alpha</t>
@@ -1119,11 +1122,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="19078818"/>
-        <c:axId val="59665933"/>
+        <c:axId val="72048405"/>
+        <c:axId val="56614215"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19078818"/>
+        <c:axId val="72048405"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1197,12 +1200,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59665933"/>
+        <c:crossAx val="56614215"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59665933"/>
+        <c:axId val="56614215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +1287,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19078818"/>
+        <c:crossAx val="72048405"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2053,11 +2056,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="86286457"/>
-        <c:axId val="17831062"/>
+        <c:axId val="95056154"/>
+        <c:axId val="31351361"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86286457"/>
+        <c:axId val="95056154"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2131,12 +2134,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17831062"/>
+        <c:crossAx val="31351361"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17831062"/>
+        <c:axId val="31351361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,7 +2221,941 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86286457"/>
+        <c:crossAx val="95056154"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Carga RL Lampada 57 Ohm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>g!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>média</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>g!$A$3:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>178</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>g!$M$3:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>g!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>média teórica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>g!$A$3:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>178</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>g!$O$3:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>120.884072552598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>119.120136634208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114.911830997511</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110.456676768616</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104.41032533634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.956752856745</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.3229369199239</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.7721572613198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68.5963302918075</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>58.1076866431978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.6301474834398</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37.4907849689633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.0117404499031</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.5028584921632</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.2548890066768</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.53175527765897</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5553380867847</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.453408738800591</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0052673031773205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>g!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>g!$A$3:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>178</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>g!$N$3:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>g!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rms teórica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>g!$A$3:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>178</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>g!$P$3:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>135.464571368764</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.754729720277</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.532713806178</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>141.258711164597</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>138.896663645811</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135.237089268932</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130.169671538002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>123.685932076358</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>115.878403453006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>106.937834393698</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>97.148967062179</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>86.8837551484617</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>76.5869998305355</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>66.7400763009217</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>57.7690906039182</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.8329739983578</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42.3779483734596</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.0027133148832</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.6926318602112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="32442802"/>
+        <c:axId val="62888168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="32442802"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="180"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>alpha (º)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="62888168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="62888168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tensão (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32442802"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2262,13 +3199,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>88920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>554760</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2276,8 +3213,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="88920" y="3884760"/>
-        <a:ext cx="5761440" cy="3232080"/>
+        <a:off x="88920" y="3980880"/>
+        <a:ext cx="5761440" cy="3231720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2289,16 +3226,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>337680</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>432720</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>565200</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>97920</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2306,12 +3243,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7595640" y="3972600"/>
-        <a:ext cx="5761440" cy="3232080"/>
+        <a:off x="8652600" y="4089600"/>
+        <a:ext cx="6523200" cy="3231720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>429120</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="15841800" y="3950280"/>
+        <a:ext cx="6523200" cy="3231720"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2325,10 +3292,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S29" activeCellId="0" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2356,40 +3323,58 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="P2" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2428,8 +3413,26 @@
         <v>0.034906585039887</v>
       </c>
       <c r="K3" s="0" t="n">
+        <f aca="false">L3</f>
+        <v>0.0349065850398866</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <f aca="false">A3*PI()/180</f>
         <v>0.0349065850398866</v>
+      </c>
+      <c r="M3" s="11" t="n">
+        <v>117</v>
+      </c>
+      <c r="N3" s="10" t="n">
+        <v>131</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K3)+ COS(A3*PI()/180))/PI()</f>
+        <v>120.884072552598</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K3 - SIN(PI() + K3)/2 + SIN(2*A3*PI()/180)/2 - A3*PI()/180))/SQRT(2*PI())</f>
+        <v>135.464571368764</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2467,12 +3470,30 @@
       <c r="J4" s="12" t="n">
         <v>0.174532925199433</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="12" t="n">
+        <f aca="false">L4</f>
+        <v>0.174532925199433</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <f aca="false">A4*PI()/180</f>
         <v>0.174532925199433</v>
       </c>
+      <c r="M4" s="11" t="n">
+        <v>116</v>
+      </c>
+      <c r="N4" s="10" t="n">
+        <v>131</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K4)+ COS(A4*PI()/180))/PI()</f>
+        <v>119.120136634208</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K4 - SIN(PI() + K4)/2 + SIN(2*A4*PI()/180)/2 - A4*PI()/180))/SQRT(2*PI())</f>
+        <v>139.754729720277</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="n">
         <v>20</v>
       </c>
@@ -2507,9 +3528,26 @@
       <c r="J5" s="0" t="n">
         <v>0.349065850398866</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="12" t="n">
+        <v>0.282577924370546</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <f aca="false">A5*PI()/180</f>
         <v>0.349065850398866</v>
+      </c>
+      <c r="M5" s="11" t="n">
+        <v>113</v>
+      </c>
+      <c r="N5" s="10" t="n">
+        <v>131</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K5)+ COS(A5*PI()/180))/PI()</f>
+        <v>114.911830997511</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K5 - SIN(PI() + K5)/2 + SIN(2*A5*PI()/180)/2 - A5*PI()/180))/SQRT(2*PI())</f>
+        <v>142.532713806178</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,8 +3586,25 @@
         <v>0.523598775598299</v>
       </c>
       <c r="K6" s="0" t="n">
+        <v>0.282568648051516</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <f aca="false">A6*PI()/180</f>
         <v>0.523598775598299</v>
+      </c>
+      <c r="M6" s="11" t="n">
+        <v>110</v>
+      </c>
+      <c r="N6" s="10" t="n">
+        <v>130</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K6)+ COS(A6*PI()/180))/PI()</f>
+        <v>110.456676768616</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K6 - SIN(PI() + K6)/2 + SIN(2*A6*PI()/180)/2 - A6*PI()/180))/SQRT(2*PI())</f>
+        <v>141.258711164597</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2588,8 +3643,25 @@
         <v>0.698131700797732</v>
       </c>
       <c r="K7" s="0" t="n">
+        <v>0.28254582029238</v>
+      </c>
+      <c r="L7" s="0" t="n">
         <f aca="false">A7*PI()/180</f>
         <v>0.698131700797732</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>105</v>
+      </c>
+      <c r="N7" s="10" t="n">
+        <v>128</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K7)+ COS(A7*PI()/180))/PI()</f>
+        <v>104.41032533634</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K7 - SIN(PI() + K7)/2 + SIN(2*A7*PI()/180)/2 - A7*PI()/180))/SQRT(2*PI())</f>
+        <v>138.896663645811</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,8 +3700,25 @@
         <v>0.872664625997165</v>
       </c>
       <c r="K8" s="0" t="n">
+        <v>0.282494660581478</v>
+      </c>
+      <c r="L8" s="0" t="n">
         <f aca="false">A8*PI()/180</f>
         <v>0.872664625997165</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="N8" s="10" t="n">
+        <v>125</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K8)+ COS(A8*PI()/180))/PI()</f>
+        <v>96.956752856745</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K8 - SIN(PI() + K8)/2 + SIN(2*A8*PI()/180)/2 - A8*PI()/180))/SQRT(2*PI())</f>
+        <v>135.237089268932</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,8 +3757,25 @@
         <v>1.0471975511966</v>
       </c>
       <c r="K9" s="0" t="n">
+        <v>0.282386770359588</v>
+      </c>
+      <c r="L9" s="0" t="n">
         <f aca="false">A9*PI()/180</f>
         <v>1.0471975511966</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>92</v>
+      </c>
+      <c r="N9" s="10" t="n">
+        <v>121</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K9)+ COS(A9*PI()/180))/PI()</f>
+        <v>88.3229369199239</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K9 - SIN(PI() + K9)/2 + SIN(2*A9*PI()/180)/2 - A9*PI()/180))/SQRT(2*PI())</f>
+        <v>130.169671538002</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,8 +3814,25 @@
         <v>1.02192644225211</v>
       </c>
       <c r="K10" s="0" t="n">
+        <v>0.282169219017632</v>
+      </c>
+      <c r="L10" s="0" t="n">
         <f aca="false">A10*PI()/180</f>
         <v>1.22173047639603</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <v>84</v>
+      </c>
+      <c r="N10" s="10" t="n">
+        <v>115</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K10)+ COS(A10*PI()/180))/PI()</f>
+        <v>78.7721572613198</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K10 - SIN(PI() + K10)/2 + SIN(2*A10*PI()/180)/2 - A10*PI()/180))/SQRT(2*PI())</f>
+        <v>123.685932076358</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,8 +3871,25 @@
         <v>0.982086556239764</v>
       </c>
       <c r="K11" s="0" t="n">
+        <v>0.281746060978595</v>
+      </c>
+      <c r="L11" s="0" t="n">
         <f aca="false">A11*PI()/180</f>
         <v>1.39626340159546</v>
+      </c>
+      <c r="M11" s="11" t="n">
+        <v>75</v>
+      </c>
+      <c r="N11" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K11)+ COS(A11*PI()/180))/PI()</f>
+        <v>68.5963302918075</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K11 - SIN(PI() + K11)/2 + SIN(2*A11*PI()/180)/2 - A11*PI()/180))/SQRT(2*PI())</f>
+        <v>115.878403453006</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,8 +3928,25 @@
         <v>0.93418270402243</v>
       </c>
       <c r="K12" s="0" t="n">
+        <v>0.280947859147622</v>
+      </c>
+      <c r="L12" s="0" t="n">
         <f aca="false">A12*PI()/180</f>
         <v>1.5707963267949</v>
+      </c>
+      <c r="M12" s="11" t="n">
+        <v>66</v>
+      </c>
+      <c r="N12" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K12)+ COS(A12*PI()/180))/PI()</f>
+        <v>58.1076866431978</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K12 - SIN(PI() + K12)/2 + SIN(2*A12*PI()/180)/2 - A12*PI()/180))/SQRT(2*PI())</f>
+        <v>106.937834393698</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,8 +3985,25 @@
         <v>0.877534468892555</v>
       </c>
       <c r="K13" s="0" t="n">
+        <v>0.279482620506319</v>
+      </c>
+      <c r="L13" s="0" t="n">
         <f aca="false">A13*PI()/180</f>
         <v>1.74532925199433</v>
+      </c>
+      <c r="M13" s="11" t="n">
+        <v>57</v>
+      </c>
+      <c r="N13" s="10" t="n">
+        <v>93</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K13)+ COS(A13*PI()/180))/PI()</f>
+        <v>47.6301474834398</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K13 - SIN(PI() + K13)/2 + SIN(2*A13*PI()/180)/2 - A13*PI()/180))/SQRT(2*PI())</f>
+        <v>97.148967062179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,8 +4042,25 @@
         <v>0.811428674750211</v>
       </c>
       <c r="K14" s="0" t="n">
+        <v>0.276858165683221</v>
+      </c>
+      <c r="L14" s="0" t="n">
         <f aca="false">A14*PI()/180</f>
         <v>1.91986217719376</v>
+      </c>
+      <c r="M14" s="11" t="n">
+        <v>48</v>
+      </c>
+      <c r="N14" s="10" t="n">
+        <v>83</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K14)+ COS(A14*PI()/180))/PI()</f>
+        <v>37.4907849689633</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K14 - SIN(PI() + K14)/2 + SIN(2*A14*PI()/180)/2 - A14*PI()/180))/SQRT(2*PI())</f>
+        <v>86.8837551484617</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,8 +4099,25 @@
         <v>0.735096964555009</v>
       </c>
       <c r="K15" s="0" t="n">
+        <v>0.272259809635739</v>
+      </c>
+      <c r="L15" s="0" t="n">
         <f aca="false">A15*PI()/180</f>
         <v>2.0943951023932</v>
+      </c>
+      <c r="M15" s="11" t="n">
+        <v>39</v>
+      </c>
+      <c r="N15" s="10" t="n">
+        <v>73</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K15)+ COS(A15*PI()/180))/PI()</f>
+        <v>28.0117404499031</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K15 - SIN(PI() + K15)/2 + SIN(2*A15*PI()/180)/2 - A15*PI()/180))/SQRT(2*PI())</f>
+        <v>76.5869998305355</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,8 +4156,25 @@
         <v>0.647683149376233</v>
       </c>
       <c r="K16" s="0" t="n">
+        <v>0.264354017006098</v>
+      </c>
+      <c r="L16" s="0" t="n">
         <f aca="false">A16*PI()/180</f>
         <v>2.26892802759263</v>
+      </c>
+      <c r="M16" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="N16" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K16)+ COS(A16*PI()/180))/PI()</f>
+        <v>19.5028584921632</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K16 - SIN(PI() + K16)/2 + SIN(2*A16*PI()/180)/2 - A16*PI()/180))/SQRT(2*PI())</f>
+        <v>66.7400763009217</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,8 +4213,25 @@
         <v>0.548196174750787</v>
       </c>
       <c r="K17" s="0" t="n">
+        <v>0.250956510470244</v>
+      </c>
+      <c r="L17" s="0" t="n">
         <f aca="false">A17*PI()/180</f>
         <v>2.44346095279206</v>
+      </c>
+      <c r="M17" s="11" t="n">
+        <v>22</v>
+      </c>
+      <c r="N17" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K17)+ COS(A17*PI()/180))/PI()</f>
+        <v>12.2548890066768</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K17 - SIN(PI() + K17)/2 + SIN(2*A17*PI()/180)/2 - A17*PI()/180))/SQRT(2*PI())</f>
+        <v>57.7690906039182</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,8 +4270,25 @@
         <v>0.435441728780333</v>
       </c>
       <c r="K18" s="0" t="n">
+        <v>0.228417253756118</v>
+      </c>
+      <c r="L18" s="0" t="n">
         <f aca="false">A18*PI()/180</f>
         <v>2.61799387799149</v>
+      </c>
+      <c r="M18" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="N18" s="10" t="n">
+        <v>38</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K18)+ COS(A18*PI()/180))/PI()</f>
+        <v>6.53175527765897</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K18 - SIN(PI() + K18)/2 + SIN(2*A18*PI()/180)/2 - A18*PI()/180))/SQRT(2*PI())</f>
+        <v>49.8329739983578</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,8 +4327,25 @@
         <v>0.307920205634587</v>
       </c>
       <c r="K19" s="0" t="n">
+        <v>0.190316750054044</v>
+      </c>
+      <c r="L19" s="0" t="n">
         <f aca="false">A19*PI()/180</f>
         <v>2.79252680319093</v>
+      </c>
+      <c r="M19" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="N19" s="10" t="n">
+        <v>27</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K19)+ COS(A19*PI()/180))/PI()</f>
+        <v>2.5553380867847</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K19 - SIN(PI() + K19)/2 + SIN(2*A19*PI()/180)/2 - A19*PI()/180))/SQRT(2*PI())</f>
+        <v>42.3779483734596</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,11 +4384,28 @@
         <v>0.163668323529781</v>
       </c>
       <c r="K20" s="0" t="n">
+        <v>0.124138311372151</v>
+      </c>
+      <c r="L20" s="0" t="n">
         <f aca="false">A20*PI()/180</f>
         <v>2.96705972839036</v>
       </c>
+      <c r="M20" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="N20" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K20)+ COS(A20*PI()/180))/PI()</f>
+        <v>0.453408738800591</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K20 - SIN(PI() + K20)/2 + SIN(2*A20*PI()/180)/2 - A20*PI()/180))/SQRT(2*PI())</f>
+        <v>33.0027133148832</v>
+      </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
         <v>178</v>
       </c>
@@ -3148,8 +4441,25 @@
         <v>0.0344502269060808</v>
       </c>
       <c r="K21" s="0" t="n">
+        <v>0.0323148618087179</v>
+      </c>
+      <c r="L21" s="0" t="n">
         <f aca="false">A21*PI()/180</f>
         <v>3.10668606854991</v>
+      </c>
+      <c r="M21" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <f aca="false">190*(-COS(PI() + K21)+ COS(A21*PI()/180))/PI()</f>
+        <v>0.0052673031773205</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <f aca="false">(190*SQRT(PI() + K21 - SIN(PI() + K21)/2 + SIN(2*A21*PI()/180)/2 - A21*PI()/180))/SQRT(2*PI())</f>
+        <v>16.6926318602112</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3157,11 +4467,26 @@
         <f aca="false">ATAN((43.9*60*2*PI()/1000)/9.42)</f>
         <v>1.05334135573322</v>
       </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">ATAN((43.9*60*2*PI()/1000)/57)</f>
+        <v>0.28257959460136</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="0" t="n">
+        <f aca="false">H24*180/PI()</f>
+        <v>60.3520140701021</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <f aca="false">I24*180/PI()</f>
+        <v>16.1906181471757</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3181,7 +4506,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3207,7 +4532,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>